<commit_message>
Complete all the components from buck proj
</commit_message>
<xml_diff>
--- a/Altium_Library.xlsx
+++ b/Altium_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\Altium_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB4A579-105B-443E-A57A-C1ED4D749B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328B2833-550B-4BBE-B8CD-F85481553FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="9" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="Connectors" sheetId="6" r:id="rId6"/>
     <sheet name="OPAMP" sheetId="7" r:id="rId7"/>
     <sheet name="Gate Drivers" sheetId="9" r:id="rId8"/>
+    <sheet name="ICs" sheetId="10" r:id="rId9"/>
+    <sheet name="Buzzer" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,6 +60,41 @@
           </rPr>
           <t xml:space="preserve">
 RES [VALUE] [PACKAGE] [WATTS] [TOLERANCE] [VOLTAGE]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Arturo Bayangos</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F5DAC279-57F7-4008-9E1F-E8093FCE542F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Bayangos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+IC [VALUE] [PACKAGE] [BRIEF DESC
+]</t>
         </r>
       </text>
     </comment>
@@ -327,8 +364,43 @@
 </comments>
 </file>
 
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Arturo Bayangos</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2A5C9D50-4838-4BDA-BFE3-8E13A12D60D3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Bayangos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+IC [VALUE] [PACKAGE] [BRIEF DESC
+]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="273">
   <si>
     <t>Part Number</t>
   </si>
@@ -1126,15 +1198,9 @@
     <t>https://datasheet.lcsc.com/lcsc/2309071225_Microchip-Tech-MIC4605-2YM_C637550.pdf</t>
   </si>
   <si>
-    <t>ComponentLink1Decription</t>
-  </si>
-  <si>
     <t>ComponentLink1URL</t>
   </si>
   <si>
-    <t>ComponentLink2Decription</t>
-  </si>
-  <si>
     <t>ComponentLink2URL</t>
   </si>
   <si>
@@ -1145,6 +1211,84 @@
   </si>
   <si>
     <t>https://datasheet.lcsc.com/lcsc/2304140030_Ningbo-Xinlaiya-Elec--XY126V-5-0-2P_C557646.pdf</t>
+  </si>
+  <si>
+    <t>UC3843D8TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM-CONTROLLER </t>
+  </si>
+  <si>
+    <t>30V</t>
+  </si>
+  <si>
+    <t>150 ℃</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/uc3842.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1707097391176</t>
+  </si>
+  <si>
+    <t>PWM-CONTROLLER_8P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC UC3843D8TR SOIC-8 PWM-CONTROLLER </t>
+  </si>
+  <si>
+    <t>TPS62933DRLR</t>
+  </si>
+  <si>
+    <t>IC TPS62933DRLR SOT-583 BUCK-CHIP</t>
+  </si>
+  <si>
+    <t>SOT-583</t>
+  </si>
+  <si>
+    <t>BUCK-CHIP</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tps62933p.pdf?ts=1658586703977&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FTPS62933P%253Fjktype%253Dhomepageproduct</t>
+  </si>
+  <si>
+    <t>3.8V-30V</t>
+  </si>
+  <si>
+    <t>ComponentLink1Description</t>
+  </si>
+  <si>
+    <t>ComponentLink2Description</t>
+  </si>
+  <si>
+    <t>BUCK-CHIP_8P</t>
+  </si>
+  <si>
+    <t>HNB09A03</t>
+  </si>
+  <si>
+    <t>BUZZER HNB09A03 TH 1.5V-5V 3Khz</t>
+  </si>
+  <si>
+    <t>30mA</t>
+  </si>
+  <si>
+    <t>1.5V - 4.5V</t>
+  </si>
+  <si>
+    <t>20℃~+70℃</t>
+  </si>
+  <si>
+    <t>Jiangsu Huaneng Elec</t>
+  </si>
+  <si>
+    <t>BUZZER_HNB09A03</t>
+  </si>
+  <si>
+    <t>BUZZER</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1811141116_Jiangsu-Huaneng-Elec-HNB09A03_C96102.pdf</t>
   </si>
 </sst>
 </file>
@@ -1545,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCD62EA-A4C2-4822-A53B-455EB5DB279A}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1586,16 +1730,16 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
@@ -2146,12 +2290,129 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED6ABB6-CE05-4C53-85C7-114D8BE94CDA}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="33">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="90">
+      <c r="A2" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4365F3-3949-4A6B-97A2-DB0027B79608}">
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2188,16 +2449,16 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
@@ -2651,7 +2912,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2694,16 +2955,16 @@
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="45">
@@ -2833,7 +3094,7 @@
   <dimension ref="A1:Q103"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:Q1"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2842,7 +3103,7 @@
     <col min="10" max="17" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="80.25">
+    <row r="1" spans="1:17" ht="36">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2883,19 +3144,19 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="45">
+    </row>
+    <row r="2" spans="1:17" ht="90">
       <c r="A2" s="2" t="s">
         <v>164</v>
       </c>
@@ -2939,7 +3200,7 @@
         <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>20</v>
@@ -3197,7 +3458,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:Q1"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3246,16 +3507,16 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="90">
@@ -3302,7 +3563,7 @@
         <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>20</v>
@@ -3366,129 +3627,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="17" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="78.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="45">
-      <c r="A2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H2" t="s">
-        <v>205</v>
-      </c>
-      <c r="I2" t="s">
-        <v>206</v>
-      </c>
-      <c r="J2" t="s">
-        <v>207</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>208</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" t="s">
-        <v>248</v>
-      </c>
-      <c r="P2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA596F63-079D-460A-9588-89767C800467}">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="N1" sqref="N1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3510,6 +3649,128 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="45">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>208</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>246</v>
+      </c>
+      <c r="P2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA596F63-079D-460A-9588-89767C800467}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="19" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="31.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>211</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -3543,13 +3804,19 @@
         <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>19</v>
+        <v>261</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="75">
+        <v>242</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="75">
       <c r="A2" s="2" t="s">
         <v>209</v>
       </c>
@@ -3596,9 +3863,14 @@
         <v>7</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="Q2" s="2"/>
+      <c r="R2" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3608,18 +3880,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2131FB0C-6EC1-4E51-BEF2-D849CF3EFF3A}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="17" width="20.7109375" customWidth="1"/>
+    <col min="1" max="19" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="33">
+    <row r="1" spans="1:19" ht="33">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3666,13 +3938,19 @@
         <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="75">
+    <row r="2" spans="1:19" ht="75">
       <c r="A2" s="2" t="s">
         <v>225</v>
       </c>
@@ -3723,6 +4001,172 @@
       </c>
       <c r="Q2" s="2" t="s">
         <v>241</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4003CD7C-8392-43D4-A280-6A4E621E0B99}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="33">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="105">
+      <c r="A2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="135">
+      <c r="A3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I3" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>263</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add USB-C and UBC Mini-B
</commit_message>
<xml_diff>
--- a/Altium_Library.xlsx
+++ b/Altium_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\Altium_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12342D4D-F26A-4954-859F-D937B51A8C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FDBA81-B7FC-4AB3-A6CF-0C929C75137D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="1" activeTab="12" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="1" activeTab="4" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="394">
   <si>
     <t>Part Number</t>
   </si>
@@ -598,9 +598,6 @@
   </si>
   <si>
     <t>0604</t>
-  </si>
-  <si>
-    <t>RES_0604</t>
   </si>
   <si>
     <t>YAGEO</t>
@@ -1649,12 +1646,171 @@
   <si>
     <t>https://datasheet.lcsc.com/lcsc/2304140030_BRIGHT-TSA063G60-250_C294566.pdf</t>
   </si>
+  <si>
+    <t>RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>RES 100K 0603 1% 0.1W 75V</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1809281124_YAGEO-RC0603FR-07100KL_C14675.pdf</t>
+  </si>
+  <si>
+    <t>RC0603FR-0727KL</t>
+  </si>
+  <si>
+    <t>RES 27K 0603 1% 0.1W 75V</t>
+  </si>
+  <si>
+    <t>27K</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_YAGEO-RC0603FR-0727KL_C114614.pdf</t>
+  </si>
+  <si>
+    <t>RC0603FR-073K9L</t>
+  </si>
+  <si>
+    <t>RES 3K9 0603 1% 0.1W 75V</t>
+  </si>
+  <si>
+    <t>3K9</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_YAGEO-RC0603FR-073K9L_C114616.pdf</t>
+  </si>
+  <si>
+    <t>F185-1106A0ASUC2</t>
+  </si>
+  <si>
+    <t>CONN F185-1106A0ASUC2 TH 2.54mm 1X6P</t>
+  </si>
+  <si>
+    <t>2.54mm</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>1X6P</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2401051806_Yxcon-F185-1106A0ASUC2_C20071199.pdf</t>
+  </si>
+  <si>
+    <t>Yxcon</t>
+  </si>
+  <si>
+    <t>HEADER_1X6P_2.54mm</t>
+  </si>
+  <si>
+    <t>FEMALE_HEADER_6P_2.54mm</t>
+  </si>
+  <si>
+    <t>F185-1108A0ASUE4</t>
+  </si>
+  <si>
+    <t>CONN F185-1108A0ASUE4 TH 2.54mm 1X8P</t>
+  </si>
+  <si>
+    <t>1X8P</t>
+  </si>
+  <si>
+    <t>FEMALE_HEADER_8P_2.54mm</t>
+  </si>
+  <si>
+    <t>HEADER_1X8P_2.54mm</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2312291746_Yxcon-F185-1108A0ASUE4_C20071201.pdf</t>
+  </si>
+  <si>
+    <t>0402WGF0000TCE</t>
+  </si>
+  <si>
+    <t>RES 0R 0402 1% 0.625W</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(Uniroyal Elec)</t>
+  </si>
+  <si>
+    <t>RES_0402</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2206010216_UNI-ROYAL-Uniroyal-Elec-0402WGF0000TCE_C17168.pdf</t>
+  </si>
+  <si>
+    <t>CC0603JRNPO9BN360</t>
+  </si>
+  <si>
+    <t>CAP 36P 0402 NPO 50V 5%</t>
+  </si>
+  <si>
+    <t>36P</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_YAGEO-CC0603JRNPO9BN360_C134070.pdf</t>
+  </si>
+  <si>
+    <t>TYPEC-304-ACP16</t>
+  </si>
+  <si>
+    <t>CONN TYPEC-304-ACP16 SMD USB-C 2.0</t>
+  </si>
+  <si>
+    <t>USB-C</t>
+  </si>
+  <si>
+    <t>Supported protocol</t>
+  </si>
+  <si>
+    <t>USB 2.0</t>
+  </si>
+  <si>
+    <t>XUNPU</t>
+  </si>
+  <si>
+    <t>USB-C_2.0</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2203111830_XUNPU-TYPEC-304-ACP16_C2982555.pdf</t>
+  </si>
+  <si>
+    <t>USB-C_2.0_12PIN</t>
+  </si>
+  <si>
+    <t>UX-144S-ACP5</t>
+  </si>
+  <si>
+    <t>CONN UX-144S-ACP5 SMD USB_Mini-B 2.0</t>
+  </si>
+  <si>
+    <t>1.5A</t>
+  </si>
+  <si>
+    <t>USB Mini-B</t>
+  </si>
+  <si>
+    <t>USB_Mini-B</t>
+  </si>
+  <si>
+    <t>USB_Mini-B_UX-144S-ACP5</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2008122036_XUNPU-UX-144S-ACP5_C720611.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1673,11 +1829,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="HarmonyOS Sans SC"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1720,7 +1871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1728,7 +1879,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2048,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCD62EA-A4C2-4822-A53B-455EB5DB279A}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2089,16 +2239,16 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
@@ -2191,10 +2341,10 @@
         <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -2209,7 +2359,7 @@
         <v>19</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>20</v>
@@ -2217,22 +2367,22 @@
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -2247,7 +2397,7 @@
         <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>20</v>
@@ -2255,13 +2405,13 @@
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
@@ -2285,7 +2435,7 @@
         <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>20</v>
@@ -2293,19 +2443,19 @@
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
@@ -2323,7 +2473,7 @@
         <v>19</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>20</v>
@@ -2331,19 +2481,19 @@
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>17</v>
@@ -2361,7 +2511,7 @@
         <v>19</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>20</v>
@@ -2369,19 +2519,19 @@
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>17</v>
@@ -2399,7 +2549,7 @@
         <v>19</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>20</v>
@@ -2407,28 +2557,28 @@
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>7</v>
@@ -2437,7 +2587,7 @@
         <v>19</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>20</v>
@@ -2445,19 +2595,19 @@
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
@@ -2475,7 +2625,7 @@
         <v>19</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>20</v>
@@ -2483,19 +2633,19 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
@@ -2513,7 +2663,7 @@
         <v>19</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>20</v>
@@ -2521,19 +2671,19 @@
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
@@ -2551,7 +2701,7 @@
         <v>19</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>20</v>
@@ -2559,13 +2709,13 @@
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>15</v>
@@ -2589,30 +2739,175 @@
         <v>19</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" customHeight="1"/>
-    <row r="16" spans="1:13" ht="30" customHeight="1"/>
-    <row r="17" ht="30" customHeight="1"/>
-    <row r="18" ht="30" customHeight="1"/>
-    <row r="19" ht="30" customHeight="1"/>
-    <row r="20" ht="30" customHeight="1"/>
-    <row r="21" ht="30" customHeight="1"/>
-    <row r="22" ht="30" customHeight="1"/>
-    <row r="23" ht="30" customHeight="1"/>
-    <row r="24" ht="30" customHeight="1"/>
-    <row r="25" ht="30" customHeight="1"/>
-    <row r="26" ht="30" customHeight="1"/>
-    <row r="27" ht="30" customHeight="1"/>
-    <row r="28" ht="30" customHeight="1"/>
-    <row r="29" ht="30" customHeight="1"/>
-    <row r="30" ht="30" customHeight="1"/>
-    <row r="31" ht="30" customHeight="1"/>
-    <row r="32" ht="30" customHeight="1"/>
+    <row r="15" spans="1:13" ht="30" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D18" s="2">
+        <v>402</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1"/>
+    <row r="20" spans="1:12" ht="30" customHeight="1"/>
+    <row r="21" spans="1:12" ht="30" customHeight="1"/>
+    <row r="22" spans="1:12" ht="30" customHeight="1"/>
+    <row r="23" spans="1:12" ht="30" customHeight="1"/>
+    <row r="24" spans="1:12" ht="30" customHeight="1"/>
+    <row r="25" spans="1:12" ht="30" customHeight="1"/>
+    <row r="26" spans="1:12" ht="30" customHeight="1"/>
+    <row r="27" spans="1:12" ht="30" customHeight="1"/>
+    <row r="28" spans="1:12" ht="30" customHeight="1"/>
+    <row r="29" spans="1:12" ht="30" customHeight="1"/>
+    <row r="30" spans="1:12" ht="30" customHeight="1"/>
+    <row r="31" spans="1:12" ht="30" customHeight="1"/>
+    <row r="32" spans="1:12" ht="30" customHeight="1"/>
     <row r="33" ht="30" customHeight="1"/>
     <row r="34" ht="30" customHeight="1"/>
     <row r="35" ht="30" customHeight="1"/>
@@ -2645,7 +2940,8 @@
     <hyperlink ref="K10" r:id="rId5" xr:uid="{76B7D361-ACA6-4D43-9341-1776B6875168}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -2676,13 +2972,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
@@ -2700,51 +2996,51 @@
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="90">
       <c r="A2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>7</v>
@@ -2753,7 +3049,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>20</v>
@@ -2793,19 +3089,19 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2823,57 +3119,57 @@
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="75">
       <c r="A2" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>7</v>
@@ -2882,7 +3178,7 @@
         <v>19</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -2920,28 +3216,28 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -2959,66 +3255,66 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="75">
       <c r="A2" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" t="s">
+        <v>311</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="J2" t="s">
-        <v>312</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>7</v>
@@ -3027,59 +3323,59 @@
         <v>19</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21" ht="75">
       <c r="A3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C3" t="s">
-        <v>317</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" t="s">
         <v>319</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" t="s">
         <v>321</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>322</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>323</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K3" t="s">
         <v>324</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="K3" t="s">
-        <v>325</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" t="s">
         <v>327</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>7</v>
@@ -3088,7 +3384,7 @@
         <v>19</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -3101,7 +3397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB2BB18-3FA8-4D14-8582-EC96300C127A}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -3124,16 +3420,16 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>12</v>
@@ -3151,54 +3447,54 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="45">
+    </row>
+    <row r="2" spans="1:17" ht="60">
       <c r="A2" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>7</v>
@@ -3207,7 +3503,7 @@
         <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -3223,7 +3519,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3260,42 +3556,42 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>7</v>
@@ -3304,39 +3600,39 @@
         <v>19</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>7</v>
@@ -3345,39 +3641,39 @@
         <v>19</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="D4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>7</v>
@@ -3386,39 +3682,39 @@
         <v>19</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>7</v>
@@ -3427,39 +3723,39 @@
         <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>7</v>
@@ -3468,7 +3764,7 @@
         <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>20</v>
@@ -3477,28 +3773,28 @@
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>7</v>
@@ -3507,7 +3803,7 @@
         <v>19</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>20</v>
@@ -3516,28 +3812,28 @@
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>7</v>
@@ -3546,39 +3842,39 @@
         <v>19</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>7</v>
@@ -3587,7 +3883,7 @@
         <v>19</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>20</v>
@@ -3596,28 +3892,28 @@
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>7</v>
@@ -3626,7 +3922,7 @@
         <v>19</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>20</v>
@@ -3634,29 +3930,29 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>7</v>
@@ -3664,11 +3960,49 @@
       <c r="J11" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" ht="30" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D12" s="2">
+        <v>402</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
     <row r="13" spans="1:13" ht="30" customHeight="1"/>
     <row r="14" spans="1:13" ht="30" customHeight="1"/>
     <row r="15" spans="1:13" ht="30" customHeight="1"/>
@@ -3742,10 +4076,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -3766,48 +4100,48 @@
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="45">
       <c r="A2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>7</v>
@@ -3822,34 +4156,34 @@
     </row>
     <row r="3" spans="1:15" ht="45">
       <c r="A3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>7</v>
@@ -3858,35 +4192,35 @@
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>7</v>
@@ -3928,16 +4262,16 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>12</v>
@@ -3955,54 +4289,54 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="90">
       <c r="A2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>7</v>
@@ -4011,7 +4345,7 @@
         <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>20</v>
@@ -4266,18 +4600,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5197523-F574-4789-9845-687AB35A38BD}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="17" width="20.7109375" customWidth="1"/>
+    <col min="1" max="18" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="31.5">
+    <row r="1" spans="1:18" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4291,93 +4625,301 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="45">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>199</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" t="s">
         <v>202</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" t="s">
         <v>204</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="45">
-      <c r="A2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J2" t="s">
         <v>205</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>206</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>207</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="75">
+      <c r="A3" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" t="s">
-        <v>208</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="M3" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O3" t="s">
         <v>19</v>
       </c>
-      <c r="O2" t="s">
-        <v>246</v>
-      </c>
-      <c r="P2" t="s">
-        <v>20</v>
+      <c r="P3" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" ht="75">
+      <c r="A4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F4" t="s">
+        <v>324</v>
+      </c>
+      <c r="G4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H4" t="s">
+        <v>364</v>
+      </c>
+      <c r="I4" t="s">
+        <v>324</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="60">
+      <c r="A5" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="60">
+      <c r="A6" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -4413,16 +4955,16 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>12</v>
@@ -4440,54 +4982,54 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="90">
       <c r="A2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="F2" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" t="s">
         <v>179</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H2" t="s">
-        <v>180</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>7</v>
@@ -4496,7 +5038,7 @@
         <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>20</v>
@@ -4504,40 +5046,40 @@
     </row>
     <row r="3" spans="1:17" ht="60">
       <c r="A3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="H3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>7</v>
@@ -4546,7 +5088,7 @@
         <v>19</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4582,22 +5124,22 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
@@ -4615,60 +5157,60 @@
         <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="75">
       <c r="A2" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>7</v>
@@ -4677,7 +5219,7 @@
         <v>19</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>20</v>
@@ -4716,22 +5258,22 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
@@ -4749,60 +5291,60 @@
         <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="75">
       <c r="A2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="J2" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>7</v>
@@ -4811,7 +5353,7 @@
         <v>19</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>20</v>
@@ -4850,13 +5392,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
@@ -4874,51 +5416,51 @@
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="105">
       <c r="A2" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>7</v>
@@ -4927,7 +5469,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>20</v>
@@ -4935,37 +5477,37 @@
     </row>
     <row r="3" spans="1:16" ht="135">
       <c r="A3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" t="s">
         <v>256</v>
       </c>
-      <c r="C3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>257</v>
       </c>
-      <c r="E3" t="s">
-        <v>258</v>
-      </c>
       <c r="F3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="I3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>7</v>
@@ -4974,7 +5516,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>20</v>
@@ -4982,37 +5524,37 @@
     </row>
     <row r="4" spans="1:16" ht="75">
       <c r="A4" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G4" t="s">
+        <v>277</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="G4" t="s">
-        <v>278</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>7</v>
@@ -5021,7 +5563,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Add 5K1 0402 for UCB-C, CC pins
</commit_message>
<xml_diff>
--- a/Altium_Library.xlsx
+++ b/Altium_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\Altium_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FDBA81-B7FC-4AB3-A6CF-0C929C75137D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D89D465-843B-4592-89A0-5292275FB2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="1" activeTab="4" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="398">
   <si>
     <t>Part Number</t>
   </si>
@@ -1804,6 +1804,18 @@
   </si>
   <si>
     <t>https://datasheet.lcsc.com/lcsc/2008122036_XUNPU-UX-144S-ACP5_C720611.pdf</t>
+  </si>
+  <si>
+    <t>RC0402FR-075K1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 5K1 0402 1% 0.625W 50V </t>
+  </si>
+  <si>
+    <t>5K1</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_YAGEO-RC0402FR-075K1L_C105872.pdf</t>
   </si>
 </sst>
 </file>
@@ -2198,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCD62EA-A4C2-4822-A53B-455EB5DB279A}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2869,8 +2881,8 @@
       <c r="C18" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D18" s="2">
-        <v>402</v>
+      <c r="D18" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>371</v>
@@ -2893,8 +2905,43 @@
       <c r="K18" s="2" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="30" customHeight="1"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="D19" s="2">
+        <v>402</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
     <row r="20" spans="1:12" ht="30" customHeight="1"/>
     <row r="21" spans="1:12" ht="30" customHeight="1"/>
     <row r="22" spans="1:12" ht="30" customHeight="1"/>
@@ -4602,8 +4649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5197523-F574-4789-9845-687AB35A38BD}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add SW debug connectors
</commit_message>
<xml_diff>
--- a/Altium_Library.xlsx
+++ b/Altium_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\Altium_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D89D465-843B-4592-89A0-5292275FB2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EA1E56-F01F-4FE7-AAE3-60EEBA0E8E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="3" activeTab="4" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="410">
   <si>
     <t>Part Number</t>
   </si>
@@ -1686,9 +1686,6 @@
     <t>F185-1106A0ASUC2</t>
   </si>
   <si>
-    <t>CONN F185-1106A0ASUC2 TH 2.54mm 1X6P</t>
-  </si>
-  <si>
     <t>2.54mm</t>
   </si>
   <si>
@@ -1713,9 +1710,6 @@
     <t>F185-1108A0ASUE4</t>
   </si>
   <si>
-    <t>CONN F185-1108A0ASUE4 TH 2.54mm 1X8P</t>
-  </si>
-  <si>
     <t>1X8P</t>
   </si>
   <si>
@@ -1816,6 +1810,49 @@
   </si>
   <si>
     <t>https://datasheet.lcsc.com/lcsc/2304140030_YAGEO-RC0402FR-075K1L_C105872.pdf</t>
+  </si>
+  <si>
+    <t>2X5P</t>
+  </si>
+  <si>
+    <t>HEADER_2X5P_2.54mm</t>
+  </si>
+  <si>
+    <t>HDR F185-1106A0ASUC2 TH 2.54mm 1X6P</t>
+  </si>
+  <si>
+    <t>HDR F185-1108A0ASUE4 TH 2.54mm 1X8P</t>
+  </si>
+  <si>
+    <t>X9555WR-2x05-6TV01</t>
+  </si>
+  <si>
+    <t>SOCKET 
+X9555WR-2x05-6TV01 TH 2.54mm 2X5P HORZ</t>
+  </si>
+  <si>
+    <t>2X5P HORZ</t>
+  </si>
+  <si>
+    <t>XKB Connectivity</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2110112030_XKB-Connectivity-X9555WR-2x05-6TV01_C2682217.pdf</t>
+  </si>
+  <si>
+    <t>SOCKET 15477610 TH 2.54mm 2X5P</t>
+  </si>
+  <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>SOCKET_2X5P_15477610</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_MOLEX-15477610_C293309.pdf</t>
+  </si>
+  <si>
+    <t>SOCKET_2X5P_2.54mm_HORZ_X9555WR</t>
   </si>
 </sst>
 </file>
@@ -2210,7 +2247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCD62EA-A4C2-4822-A53B-455EB5DB279A}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -2873,22 +2910,22 @@
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>14</v>
@@ -2903,19 +2940,19 @@
         <v>19</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>396</v>
       </c>
       <c r="D19" s="2">
         <v>402</v>
@@ -2924,7 +2961,7 @@
         <v>30</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>14</v>
@@ -2939,7 +2976,7 @@
         <v>19</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1"/>
@@ -4015,13 +4052,13 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="D12" s="2">
         <v>402</v>
@@ -4045,7 +4082,7 @@
         <v>19</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -4647,10 +4684,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5197523-F574-4789-9845-687AB35A38BD}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4684,7 +4721,7 @@
         <v>203</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -4772,7 +4809,7 @@
         <v>353</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>354</v>
+        <v>398</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>353</v>
@@ -4781,31 +4818,31 @@
         <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>324</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>324</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>7</v>
@@ -4814,50 +4851,50 @@
         <v>19</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="75">
       <c r="A4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>363</v>
+        <v>399</v>
       </c>
       <c r="C4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F4" t="s">
         <v>324</v>
       </c>
       <c r="G4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I4" t="s">
         <v>324</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>7</v>
@@ -4866,18 +4903,18 @@
         <v>19</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="60">
       <c r="A5" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>332</v>
@@ -4889,25 +4926,25 @@
         <v>324</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>382</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>7</v>
@@ -4916,18 +4953,18 @@
         <v>19</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="60">
       <c r="A6" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>332</v>
@@ -4939,25 +4976,25 @@
         <v>324</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>7</v>
@@ -4966,7 +5003,107 @@
         <v>19</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="75">
+      <c r="A7" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="75">
+      <c r="A8">
+        <v>15477610</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C8">
+        <v>15477610</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Banana jack & RGB LED
</commit_message>
<xml_diff>
--- a/Altium_Library.xlsx
+++ b/Altium_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\Altium_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F644C0-0130-49D3-86B2-FBA002F76E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69879EA9-7796-4D26-A881-CA1EBE4E3355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="3" activeTab="13" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="3" activeTab="4" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="452">
   <si>
     <t>Part Number</t>
   </si>
@@ -1946,6 +1946,75 @@
   </si>
   <si>
     <t>https://datasheet.lcsc.com/lcsc/2006101642_Nexperia-PMEG3010EP-115_C552865.pdf</t>
+  </si>
+  <si>
+    <t>E6C0606RGBC3UDA</t>
+  </si>
+  <si>
+    <t>LED E6C0606RGBC3UDA 0603 RGB 5V 20mA</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>20mA</t>
+  </si>
+  <si>
+    <t>2.20V (max, red), 3.40V (max , green), 3.40V (max, blue)</t>
+  </si>
+  <si>
+    <t>90 ℃</t>
+  </si>
+  <si>
+    <t>EKINGLUX</t>
+  </si>
+  <si>
+    <t>LED_0603</t>
+  </si>
+  <si>
+    <t>LED_RGB_COMMON_P</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2203301730_EKINGLUX-E6C0606RGBC3UDA_C375569.pdf</t>
+  </si>
+  <si>
+    <t>24.247.2</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>32A</t>
+  </si>
+  <si>
+    <t>JACK  24.247.2 TH 4mm  VERT BLACK</t>
+  </si>
+  <si>
+    <t>VERT BLACK BANANA JACK</t>
+  </si>
+  <si>
+    <t>Changzhou Amass Elec</t>
+  </si>
+  <si>
+    <t>BANANA_JACK_BLACK_24.247.2</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Banana-Connectors-Alligator-Clips_Changzhou-Amass-Elec-24-247-2_C106272.html</t>
+  </si>
+  <si>
+    <t>24.247.1</t>
+  </si>
+  <si>
+    <t>JACK  24.247.1 TH 4mm  VERT RED</t>
+  </si>
+  <si>
+    <t>VERT RED BANANA JACK</t>
+  </si>
+  <si>
+    <t>BANANA_JACK_RED_24.247.1</t>
+  </si>
+  <si>
+    <t>JACK_1P</t>
   </si>
 </sst>
 </file>
@@ -3743,10 +3812,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901206C7-280F-4B16-9699-B948C29B981E}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H22:H23"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3810,7 +3879,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="45">
+    <row r="2" spans="1:18" ht="75">
       <c r="A2" s="2" t="s">
         <v>419</v>
       </c>
@@ -3862,9 +3931,60 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
+    <row r="3" spans="1:18" ht="75">
+      <c r="A3" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4954,10 +5074,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5197523-F574-4789-9845-687AB35A38BD}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5374,6 +5494,106 @@
       </c>
       <c r="P8" s="2" t="s">
         <v>408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="105">
+      <c r="A9" t="s">
+        <v>439</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C9" t="s">
+        <v>439</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="J9" t="s">
+        <v>444</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" t="s">
+        <v>451</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="105">
+      <c r="A10" t="s">
+        <v>447</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C10" t="s">
+        <v>447</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="J10" t="s">
+        <v>444</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" t="s">
+        <v>451</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some reference issues
</commit_message>
<xml_diff>
--- a/Altium_Library.xlsx
+++ b/Altium_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\Altium_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69879EA9-7796-4D26-A881-CA1EBE4E3355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B5266F-F535-422A-9426-832B40617695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="3" activeTab="4" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="2" activeTab="14" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="Crystals" sheetId="12" r:id="rId12"/>
     <sheet name="Switches" sheetId="14" r:id="rId13"/>
     <sheet name="Diodes" sheetId="15" r:id="rId14"/>
+    <sheet name="Module" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -218,6 +219,41 @@
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{51730D32-F541-4CF8-9467-84A1FC06D430}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arturo Bayangos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+IC [VALUE] [PACKAGE] [BRIEF DESC
+]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Arturo Bayangos</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D01347DE-82C8-431F-8A29-B2E19073B809}">
       <text>
         <r>
           <rPr>
@@ -544,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="463">
   <si>
     <t>Part Number</t>
   </si>
@@ -631,9 +667,6 @@
   </si>
   <si>
     <t>100R</t>
-  </si>
-  <si>
-    <t>0604</t>
   </si>
   <si>
     <t>YAGEO</t>
@@ -2015,6 +2048,42 @@
   </si>
   <si>
     <t>JACK_1P</t>
+  </si>
+  <si>
+    <t>TC0250B1052TCC</t>
+  </si>
+  <si>
+    <t>RES 10K5 0402 0.1% 0.625W 25V</t>
+  </si>
+  <si>
+    <t>10K5</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_UNI-ROYAL-Uniroyal-Elec-TC0250B1052TCC_C517521.pdf</t>
+  </si>
+  <si>
+    <t>AR02BTC5001</t>
+  </si>
+  <si>
+    <t>RES 5K 0402 0.1% 0.63W</t>
+  </si>
+  <si>
+    <t>5K</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2311271515_Viking-Tech-AR02BTC5001_C5948099.pdf</t>
+  </si>
+  <si>
+    <t>LCD_16X2_Arduino_Shield</t>
+  </si>
+  <si>
+    <t>LCD Display 16X2 Arduino Shield</t>
+  </si>
+  <si>
+    <t>LCD 16X2</t>
+  </si>
+  <si>
+    <t>LCD_MODULE_16X2</t>
   </si>
 </sst>
 </file>
@@ -2409,8 +2478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCD62EA-A4C2-4822-A53B-455EB5DB279A}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2450,16 +2519,16 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
@@ -2510,7 +2579,7 @@
       <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -2548,11 +2617,11 @@
       <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>17</v>
@@ -2570,7 +2639,7 @@
         <v>19</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>20</v>
@@ -2578,22 +2647,22 @@
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -2608,7 +2677,7 @@
         <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>20</v>
@@ -2616,13 +2685,13 @@
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
@@ -2646,7 +2715,7 @@
         <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>20</v>
@@ -2654,19 +2723,19 @@
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
@@ -2684,7 +2753,7 @@
         <v>19</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>20</v>
@@ -2692,19 +2761,19 @@
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>17</v>
@@ -2722,7 +2791,7 @@
         <v>19</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>20</v>
@@ -2730,19 +2799,19 @@
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>17</v>
@@ -2760,7 +2829,7 @@
         <v>19</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>20</v>
@@ -2768,28 +2837,28 @@
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>7</v>
@@ -2798,7 +2867,7 @@
         <v>19</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>20</v>
@@ -2806,19 +2875,19 @@
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
@@ -2836,7 +2905,7 @@
         <v>19</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>20</v>
@@ -2844,19 +2913,19 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
@@ -2874,7 +2943,7 @@
         <v>19</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>20</v>
@@ -2882,19 +2951,19 @@
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
@@ -2912,7 +2981,7 @@
         <v>19</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>20</v>
@@ -2920,13 +2989,13 @@
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>15</v>
@@ -2950,7 +3019,7 @@
         <v>19</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>20</v>
@@ -2958,19 +3027,19 @@
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1">
       <c r="A15" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
@@ -2988,7 +3057,7 @@
         <v>19</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>20</v>
@@ -2996,19 +3065,19 @@
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1">
       <c r="A16" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>17</v>
@@ -3026,7 +3095,7 @@
         <v>19</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>20</v>
@@ -3034,19 +3103,19 @@
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>17</v>
@@ -3064,7 +3133,7 @@
         <v>19</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>20</v>
@@ -3072,22 +3141,22 @@
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>14</v>
@@ -3102,28 +3171,28 @@
         <v>19</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D19" s="2">
-        <v>402</v>
+      <c r="D19" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>14</v>
@@ -3138,11 +3207,79 @@
         <v>19</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" customHeight="1"/>
-    <row r="21" spans="1:12" ht="30" customHeight="1"/>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="30" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
     <row r="22" spans="1:12" ht="30" customHeight="1"/>
     <row r="23" spans="1:12" ht="30" customHeight="1"/>
     <row r="24" spans="1:12" ht="30" customHeight="1"/>
@@ -3218,13 +3355,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
@@ -3242,51 +3379,51 @@
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="90">
       <c r="A2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>7</v>
@@ -3295,7 +3432,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>20</v>
@@ -3312,8 +3449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA19259-A477-4ADE-89DC-CBC18E6FB933}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3335,19 +3472,19 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3365,57 +3502,57 @@
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="75">
       <c r="A2" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>286</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>283</v>
+        <v>208</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>7</v>
@@ -3424,50 +3561,50 @@
         <v>19</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="75">
       <c r="A3" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D3" t="s">
         <v>411</v>
       </c>
-      <c r="C3" t="s">
-        <v>410</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>412</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H3" t="s">
         <v>414</v>
       </c>
-      <c r="G3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>415</v>
       </c>
-      <c r="I3" t="s">
-        <v>416</v>
-      </c>
       <c r="J3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>7</v>
@@ -3476,7 +3613,7 @@
         <v>19</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -3512,28 +3649,28 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -3551,66 +3688,66 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="75">
       <c r="A2" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="J2" t="s">
-        <v>311</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>7</v>
@@ -3619,59 +3756,59 @@
         <v>19</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21" ht="75">
       <c r="A3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C3" t="s">
-        <v>316</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" t="s">
         <v>318</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" t="s">
         <v>320</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>321</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>322</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>324</v>
+      </c>
+      <c r="K3" t="s">
         <v>323</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K3" t="s">
-        <v>324</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" t="s">
         <v>326</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>328</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>7</v>
@@ -3680,7 +3817,7 @@
         <v>19</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -3716,16 +3853,16 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>12</v>
@@ -3743,54 +3880,54 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="60">
       <c r="A2" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>7</v>
@@ -3799,7 +3936,7 @@
         <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -3814,8 +3951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901206C7-280F-4B16-9699-B948C29B981E}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3837,19 +3974,19 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3867,57 +4004,57 @@
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="75">
       <c r="A2" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>423</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>426</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>7</v>
@@ -3926,50 +4063,50 @@
         <v>19</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="75">
       <c r="A3" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>430</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>7</v>
@@ -3978,13 +4115,98 @@
         <v>19</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD9027B-23A1-4886-A8CA-887977C04A6F}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="11" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="31.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30">
+      <c r="A2" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4030,42 +4252,42 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>7</v>
@@ -4074,39 +4296,39 @@
         <v>19</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>7</v>
@@ -4115,39 +4337,39 @@
         <v>19</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>7</v>
@@ -4156,39 +4378,39 @@
         <v>19</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="D5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>7</v>
@@ -4197,39 +4419,39 @@
         <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>7</v>
@@ -4238,7 +4460,7 @@
         <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>20</v>
@@ -4247,28 +4469,28 @@
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>7</v>
@@ -4277,7 +4499,7 @@
         <v>19</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>20</v>
@@ -4286,28 +4508,28 @@
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>7</v>
@@ -4316,39 +4538,39 @@
         <v>19</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>7</v>
@@ -4357,7 +4579,7 @@
         <v>19</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>20</v>
@@ -4366,28 +4588,28 @@
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>7</v>
@@ -4396,7 +4618,7 @@
         <v>19</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>20</v>
@@ -4405,28 +4627,28 @@
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>7</v>
@@ -4442,28 +4664,28 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="D12" s="2">
         <v>402</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>7</v>
@@ -4472,7 +4694,7 @@
         <v>19</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -4550,10 +4772,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -4574,48 +4796,48 @@
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="45">
       <c r="A2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>7</v>
@@ -4630,34 +4852,34 @@
     </row>
     <row r="3" spans="1:15" ht="45">
       <c r="A3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>7</v>
@@ -4667,34 +4889,34 @@
     </row>
     <row r="4" spans="1:15" ht="45">
       <c r="A4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>7</v>
@@ -4736,16 +4958,16 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>12</v>
@@ -4763,54 +4985,54 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="90">
       <c r="A2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>7</v>
@@ -4819,7 +5041,7 @@
         <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>20</v>
@@ -5076,7 +5298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5197523-F574-4789-9845-687AB35A38BD}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D7" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -5099,19 +5321,19 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -5129,57 +5351,57 @@
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="45">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" t="s">
         <v>199</v>
       </c>
-      <c r="F2" t="s">
-        <v>200</v>
-      </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" t="s">
+        <v>323</v>
+      </c>
+      <c r="J2" t="s">
         <v>204</v>
       </c>
-      <c r="I2" t="s">
-        <v>324</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>205</v>
-      </c>
-      <c r="K2" t="s">
-        <v>206</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>7</v>
@@ -5188,7 +5410,7 @@
         <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q2" t="s">
         <v>20</v>
@@ -5196,43 +5418,43 @@
     </row>
     <row r="3" spans="1:18" ht="75">
       <c r="A3" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>356</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>7</v>
@@ -5241,50 +5463,50 @@
         <v>19</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="75">
       <c r="A4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F4" t="s">
+        <v>323</v>
+      </c>
+      <c r="G4" t="s">
+        <v>354</v>
+      </c>
+      <c r="H4" t="s">
         <v>361</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="C4" t="s">
-        <v>361</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>354</v>
-      </c>
-      <c r="F4" t="s">
-        <v>324</v>
-      </c>
-      <c r="G4" t="s">
-        <v>355</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>323</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="I4" t="s">
-        <v>324</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>363</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>7</v>
@@ -5293,48 +5515,48 @@
         <v>19</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="60">
       <c r="A5" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>378</v>
-      </c>
       <c r="I5" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>381</v>
-      </c>
       <c r="K5" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>7</v>
@@ -5343,48 +5565,48 @@
         <v>19</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="60">
       <c r="A6" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>388</v>
-      </c>
       <c r="I6" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>381</v>
-      </c>
       <c r="K6" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>7</v>
@@ -5393,48 +5615,48 @@
         <v>19</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="75">
       <c r="A7" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>403</v>
-      </c>
       <c r="K7" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>7</v>
@@ -5443,7 +5665,7 @@
         <v>19</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="75">
@@ -5451,40 +5673,40 @@
         <v>15477610</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C8">
         <v>15477610</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>7</v>
@@ -5493,48 +5715,48 @@
         <v>19</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="105">
       <c r="A9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C9" t="s">
+        <v>438</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="C9" t="s">
+      <c r="I9" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="J9" t="s">
         <v>443</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="K9" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>7</v>
@@ -5543,48 +5765,48 @@
         <v>19</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="105">
       <c r="A10" t="s">
+        <v>446</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" t="s">
+        <v>446</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C10" t="s">
-        <v>447</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="J10" t="s">
+        <v>443</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>449</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="J10" t="s">
-        <v>444</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>450</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>7</v>
@@ -5593,7 +5815,7 @@
         <v>19</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -5629,16 +5851,16 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>12</v>
@@ -5656,54 +5878,54 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="90">
       <c r="A2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="F2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H2" t="s">
         <v>178</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="H2" t="s">
-        <v>179</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>7</v>
@@ -5712,7 +5934,7 @@
         <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>20</v>
@@ -5720,40 +5942,40 @@
     </row>
     <row r="3" spans="1:17" ht="60">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="H3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>7</v>
@@ -5762,7 +5984,7 @@
         <v>19</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -5798,22 +6020,22 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
@@ -5831,60 +6053,60 @@
         <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="75">
       <c r="A2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>7</v>
@@ -5893,7 +6115,7 @@
         <v>19</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>20</v>
@@ -5932,22 +6154,22 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
@@ -5965,60 +6187,60 @@
         <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="75">
       <c r="A2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="G2" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="J2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>7</v>
@@ -6027,7 +6249,7 @@
         <v>19</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>20</v>
@@ -6066,13 +6288,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
@@ -6090,51 +6312,51 @@
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="105">
       <c r="A2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>7</v>
@@ -6143,7 +6365,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>20</v>
@@ -6151,37 +6373,37 @@
     </row>
     <row r="3" spans="1:16" ht="135">
       <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" t="s">
         <v>255</v>
       </c>
-      <c r="C3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>256</v>
       </c>
-      <c r="E3" t="s">
-        <v>257</v>
-      </c>
       <c r="F3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="I3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>7</v>
@@ -6190,7 +6412,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>20</v>
@@ -6198,37 +6420,37 @@
     </row>
     <row r="4" spans="1:16" ht="75">
       <c r="A4" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G4" t="s">
+        <v>276</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="G4" t="s">
-        <v>277</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>273</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>7</v>
@@ -6237,7 +6459,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Add molex connector and barrel jack
</commit_message>
<xml_diff>
--- a/Altium_Library.xlsx
+++ b/Altium_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\Altium_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B5266F-F535-422A-9426-832B40617695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1745048-DCE9-45CA-B1BF-3D34EA4F8924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="2" activeTab="14" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="2" activeTab="4" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="477">
   <si>
     <t>Part Number</t>
   </si>
@@ -2084,6 +2084,49 @@
   </si>
   <si>
     <t>LCD_MODULE_16X2</t>
+  </si>
+  <si>
+    <t>DC-058A-D010</t>
+  </si>
+  <si>
+    <t>JACK 
+DC-058A-D010 TH  HORIZ</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>HORZ 2WIRE Jack</t>
+  </si>
+  <si>
+    <t>G-Switch</t>
+  </si>
+  <si>
+    <t>CON_DC-058A-D010</t>
+  </si>
+  <si>
+    <t>JACK_2P</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2102241737_G-Switch-DC-058A-D010_C2686970.pdf</t>
+  </si>
+  <si>
+    <t>RECEP 436500200 TH 3mm HORIZ</t>
+  </si>
+  <si>
+    <t>8.5A</t>
+  </si>
+  <si>
+    <t>600V</t>
+  </si>
+  <si>
+    <t>RERCEP 2WIRE HORIZ</t>
+  </si>
+  <si>
+    <t>CON_436500200</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2305301754_MOLEX-436500200_C192562.pdf</t>
   </si>
 </sst>
 </file>
@@ -4129,7 +4172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD9027B-23A1-4886-A8CA-887977C04A6F}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -5296,10 +5339,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5197523-F574-4789-9845-687AB35A38BD}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5816,6 +5859,106 @@
       </c>
       <c r="P10" s="2" t="s">
         <v>445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="60">
+      <c r="A11" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="30">
+      <c r="A12" s="2">
+        <v>436500200</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C12" s="2">
+        <v>436500200</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix A4 schem template parameter ref
</commit_message>
<xml_diff>
--- a/Altium_Library.xlsx
+++ b/Altium_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\Altium_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1745048-DCE9-45CA-B1BF-3D34EA4F8924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D610441-3254-4195-B884-508F0E50C3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="2" activeTab="4" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{1B08D3C9-5E03-4F0E-A6E7-09EFE3E77760}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="491">
   <si>
     <t>Part Number</t>
   </si>
@@ -2127,6 +2127,48 @@
   </si>
   <si>
     <t>https://datasheet.lcsc.com/lcsc/2305301754_MOLEX-436500200_C192562.pdf</t>
+  </si>
+  <si>
+    <t>3.81mm</t>
+  </si>
+  <si>
+    <t>160V</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>RECEP 4WIRE VERT</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>CON_1803442</t>
+  </si>
+  <si>
+    <t>JACK_4P</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2001071235_Phoenix-Contact-1803442_C480518.pdf</t>
+  </si>
+  <si>
+    <t>RECEP 1803442 TH 3.81mm HORIZ</t>
+  </si>
+  <si>
+    <t>GF063P1-B102</t>
+  </si>
+  <si>
+    <t>RES POT 1K TH 20%</t>
+  </si>
+  <si>
+    <t>Tokyo Cosmos Elec</t>
+  </si>
+  <si>
+    <t>RES_GF063P1-B102</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_Tokyo-Cosmos-Elec-GF063P1-B102_C128078.pdf</t>
   </si>
 </sst>
 </file>
@@ -2521,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCD62EA-A4C2-4822-A53B-455EB5DB279A}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3323,7 +3365,44 @@
         <v>458</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30" customHeight="1"/>
+    <row r="22" spans="1:12" ht="30" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="23" spans="1:12" ht="30" customHeight="1"/>
     <row r="24" spans="1:12" ht="30" customHeight="1"/>
     <row r="25" spans="1:12" ht="30" customHeight="1"/>
@@ -5339,10 +5418,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5197523-F574-4789-9845-687AB35A38BD}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5911,7 +5990,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30">
+    <row r="12" spans="1:18" ht="75">
       <c r="A12" s="2">
         <v>436500200</v>
       </c>
@@ -5959,6 +6038,56 @@
       </c>
       <c r="P12" s="2" t="s">
         <v>476</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="60">
+      <c r="A13" s="2">
+        <v>1803442</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1803442</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>